<commit_message>
consider pasture as agriculture, not natural land
</commit_message>
<xml_diff>
--- a/data/TabularData/CDL_NVC_AgClassMatch.xlsx
+++ b/data/TabularData/CDL_NVC_AgClassMatch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SCINetPostDoc\PollinatorVegetation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SCINetPostDoc\MergeLANDFIREandCDL\data\TabularData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C34987-2C6A-442A-A3B2-B2A536DC0364}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF2D54F-81EF-44AB-9289-1BD159229508}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NASS_classes_simple" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="150">
   <si>
     <t>VALUE</t>
   </si>
@@ -1315,8 +1315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1798,6 +1798,9 @@
       <c r="C30" t="s">
         <v>34</v>
       </c>
+      <c r="D30" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -2494,6 +2497,9 @@
       <c r="C84" t="s">
         <v>34</v>
       </c>
+      <c r="D84" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
@@ -2768,6 +2774,9 @@
       <c r="C104" t="s">
         <v>6</v>
       </c>
+      <c r="D104" t="s">
+        <v>142</v>
+      </c>
       <c r="E104" t="s">
         <v>143</v>
       </c>
@@ -3092,6 +3101,9 @@
       <c r="C125" t="s">
         <v>6</v>
       </c>
+      <c r="D125" t="s">
+        <v>142</v>
+      </c>
       <c r="E125" t="s">
         <v>143</v>
       </c>
@@ -3204,6 +3216,9 @@
       <c r="C133" t="s">
         <v>6</v>
       </c>
+      <c r="D133" t="s">
+        <v>142</v>
+      </c>
       <c r="E133" t="s">
         <v>143</v>
       </c>
@@ -3227,7 +3242,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:F1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F1048576 D134:D1048576 D126:D132 D105:D124 D2:D103" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$G$2:$G$9</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update match file to address wheat/corn issue, make plots of validation results
</commit_message>
<xml_diff>
--- a/data/TabularData/CDL_NVC_AgClassMatch.xlsx
+++ b/data/TabularData/CDL_NVC_AgClassMatch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SCINetPostDoc\MergeLANDFIREandCDL\data\TabularData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF2D54F-81EF-44AB-9289-1BD159229508}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14291B7-0E33-4356-957E-185B97B882FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NASS_classes_simple" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="150">
   <si>
     <t>VALUE</t>
   </si>
@@ -1315,8 +1315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,6 +1372,9 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
+      <c r="D3" t="s">
+        <v>146</v>
+      </c>
       <c r="E3" t="s">
         <v>143</v>
       </c>
@@ -1389,6 +1392,9 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
+      <c r="D4" t="s">
+        <v>146</v>
+      </c>
       <c r="E4" t="s">
         <v>143</v>
       </c>
@@ -1406,6 +1412,9 @@
       <c r="C5" t="s">
         <v>6</v>
       </c>
+      <c r="D5" t="s">
+        <v>146</v>
+      </c>
       <c r="E5" t="s">
         <v>143</v>
       </c>
@@ -1423,6 +1432,9 @@
       <c r="C6" t="s">
         <v>6</v>
       </c>
+      <c r="D6" t="s">
+        <v>146</v>
+      </c>
       <c r="E6" t="s">
         <v>143</v>
       </c>
@@ -1440,6 +1452,9 @@
       <c r="C7" t="s">
         <v>6</v>
       </c>
+      <c r="D7" t="s">
+        <v>146</v>
+      </c>
       <c r="E7" t="s">
         <v>143</v>
       </c>
@@ -1456,6 +1471,9 @@
       </c>
       <c r="C8" t="s">
         <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>146</v>
       </c>
       <c r="E8" t="s">
         <v>143</v>
@@ -1474,6 +1492,9 @@
       <c r="C9" t="s">
         <v>6</v>
       </c>
+      <c r="D9" t="s">
+        <v>146</v>
+      </c>
       <c r="E9" t="s">
         <v>143</v>
       </c>
@@ -1491,6 +1512,9 @@
       <c r="C10" t="s">
         <v>6</v>
       </c>
+      <c r="D10" t="s">
+        <v>146</v>
+      </c>
       <c r="E10" t="s">
         <v>143</v>
       </c>
@@ -1505,6 +1529,9 @@
       <c r="C11" t="s">
         <v>6</v>
       </c>
+      <c r="D11" t="s">
+        <v>146</v>
+      </c>
       <c r="E11" t="s">
         <v>143</v>
       </c>
@@ -1519,6 +1546,9 @@
       <c r="C12" t="s">
         <v>6</v>
       </c>
+      <c r="D12" t="s">
+        <v>146</v>
+      </c>
       <c r="E12" t="s">
         <v>143</v>
       </c>
@@ -1533,6 +1563,9 @@
       <c r="C13" t="s">
         <v>6</v>
       </c>
+      <c r="D13" t="s">
+        <v>146</v>
+      </c>
       <c r="E13" t="s">
         <v>143</v>
       </c>
@@ -1683,6 +1716,9 @@
       <c r="C22" t="s">
         <v>6</v>
       </c>
+      <c r="D22" t="s">
+        <v>146</v>
+      </c>
       <c r="E22" t="s">
         <v>143</v>
       </c>
@@ -1714,6 +1750,9 @@
       <c r="C24" t="s">
         <v>6</v>
       </c>
+      <c r="D24" t="s">
+        <v>146</v>
+      </c>
       <c r="E24" t="s">
         <v>143</v>
       </c>
@@ -1728,6 +1767,9 @@
       <c r="C25" t="s">
         <v>6</v>
       </c>
+      <c r="D25" t="s">
+        <v>146</v>
+      </c>
       <c r="E25" t="s">
         <v>143</v>
       </c>
@@ -1742,6 +1784,9 @@
       <c r="C26" t="s">
         <v>6</v>
       </c>
+      <c r="D26" t="s">
+        <v>146</v>
+      </c>
       <c r="E26" t="s">
         <v>143</v>
       </c>
@@ -1756,6 +1801,9 @@
       <c r="C27" t="s">
         <v>6</v>
       </c>
+      <c r="D27" t="s">
+        <v>146</v>
+      </c>
       <c r="E27" t="s">
         <v>143</v>
       </c>
@@ -1770,6 +1818,9 @@
       <c r="C28" t="s">
         <v>6</v>
       </c>
+      <c r="D28" t="s">
+        <v>146</v>
+      </c>
       <c r="E28" t="s">
         <v>143</v>
       </c>
@@ -1784,6 +1835,9 @@
       <c r="C29" t="s">
         <v>6</v>
       </c>
+      <c r="D29" t="s">
+        <v>146</v>
+      </c>
       <c r="E29" t="s">
         <v>143</v>
       </c>
@@ -1799,6 +1853,9 @@
         <v>34</v>
       </c>
       <c r="D30" t="s">
+        <v>146</v>
+      </c>
+      <c r="E30" t="s">
         <v>143</v>
       </c>
     </row>
@@ -1812,6 +1869,9 @@
       <c r="C31" t="s">
         <v>6</v>
       </c>
+      <c r="D31" t="s">
+        <v>146</v>
+      </c>
       <c r="E31" t="s">
         <v>143</v>
       </c>
@@ -1826,6 +1886,9 @@
       <c r="C32" t="s">
         <v>6</v>
       </c>
+      <c r="D32" t="s">
+        <v>146</v>
+      </c>
       <c r="E32" t="s">
         <v>143</v>
       </c>
@@ -1840,6 +1903,9 @@
       <c r="C33" t="s">
         <v>6</v>
       </c>
+      <c r="D33" t="s">
+        <v>146</v>
+      </c>
       <c r="E33" t="s">
         <v>143</v>
       </c>
@@ -1854,6 +1920,9 @@
       <c r="C34" t="s">
         <v>6</v>
       </c>
+      <c r="D34" t="s">
+        <v>146</v>
+      </c>
       <c r="E34" t="s">
         <v>143</v>
       </c>
@@ -1868,6 +1937,9 @@
       <c r="C35" t="s">
         <v>6</v>
       </c>
+      <c r="D35" t="s">
+        <v>146</v>
+      </c>
       <c r="E35" t="s">
         <v>143</v>
       </c>
@@ -1882,6 +1954,9 @@
       <c r="C36" t="s">
         <v>6</v>
       </c>
+      <c r="D36" t="s">
+        <v>146</v>
+      </c>
       <c r="E36" t="s">
         <v>143</v>
       </c>
@@ -1896,6 +1971,9 @@
       <c r="C37" t="s">
         <v>6</v>
       </c>
+      <c r="D37" t="s">
+        <v>146</v>
+      </c>
       <c r="E37" t="s">
         <v>143</v>
       </c>
@@ -1910,6 +1988,9 @@
       <c r="C38" t="s">
         <v>6</v>
       </c>
+      <c r="D38" t="s">
+        <v>146</v>
+      </c>
       <c r="E38" t="s">
         <v>143</v>
       </c>
@@ -1924,6 +2005,9 @@
       <c r="C39" t="s">
         <v>6</v>
       </c>
+      <c r="D39" t="s">
+        <v>146</v>
+      </c>
       <c r="E39" t="s">
         <v>143</v>
       </c>
@@ -1938,6 +2022,9 @@
       <c r="C40" t="s">
         <v>6</v>
       </c>
+      <c r="D40" t="s">
+        <v>146</v>
+      </c>
       <c r="E40" t="s">
         <v>143</v>
       </c>
@@ -1952,6 +2039,9 @@
       <c r="C41" t="s">
         <v>6</v>
       </c>
+      <c r="D41" t="s">
+        <v>146</v>
+      </c>
       <c r="E41" t="s">
         <v>143</v>
       </c>
@@ -1966,6 +2056,9 @@
       <c r="C42" t="s">
         <v>6</v>
       </c>
+      <c r="D42" t="s">
+        <v>146</v>
+      </c>
       <c r="E42" t="s">
         <v>143</v>
       </c>
@@ -1980,6 +2073,9 @@
       <c r="C43" t="s">
         <v>6</v>
       </c>
+      <c r="D43" t="s">
+        <v>146</v>
+      </c>
       <c r="E43" t="s">
         <v>143</v>
       </c>
@@ -1994,6 +2090,9 @@
       <c r="C44" t="s">
         <v>6</v>
       </c>
+      <c r="D44" t="s">
+        <v>146</v>
+      </c>
       <c r="E44" t="s">
         <v>143</v>
       </c>
@@ -2008,6 +2107,9 @@
       <c r="C45" t="s">
         <v>6</v>
       </c>
+      <c r="D45" t="s">
+        <v>146</v>
+      </c>
       <c r="E45" t="s">
         <v>143</v>
       </c>
@@ -2022,6 +2124,9 @@
       <c r="C46" t="s">
         <v>6</v>
       </c>
+      <c r="D46" t="s">
+        <v>146</v>
+      </c>
       <c r="E46" t="s">
         <v>143</v>
       </c>
@@ -2067,6 +2172,9 @@
       <c r="C49" t="s">
         <v>6</v>
       </c>
+      <c r="D49" t="s">
+        <v>146</v>
+      </c>
       <c r="E49" t="s">
         <v>143</v>
       </c>
@@ -2081,6 +2189,9 @@
       <c r="C50" t="s">
         <v>6</v>
       </c>
+      <c r="D50" t="s">
+        <v>146</v>
+      </c>
       <c r="E50" t="s">
         <v>143</v>
       </c>
@@ -2095,6 +2206,9 @@
       <c r="C51" t="s">
         <v>6</v>
       </c>
+      <c r="D51" t="s">
+        <v>146</v>
+      </c>
       <c r="E51" t="s">
         <v>143</v>
       </c>
@@ -2109,6 +2223,9 @@
       <c r="C52" t="s">
         <v>6</v>
       </c>
+      <c r="D52" t="s">
+        <v>146</v>
+      </c>
       <c r="E52" t="s">
         <v>143</v>
       </c>
@@ -2123,6 +2240,9 @@
       <c r="C53" t="s">
         <v>34</v>
       </c>
+      <c r="D53" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
@@ -3242,7 +3362,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F1048576 D134:D1048576 D126:D132 D105:D124 D2:D103" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D134:D1048576 D126:D132 D105:D124 E2:F1048576 D2:D103" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$G$2:$G$9</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>